<commit_message>
append desc to days in week
</commit_message>
<xml_diff>
--- a/timesheets/2020_timeheets.xlsx
+++ b/timesheets/2020_timeheets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11505" windowWidth="12435" xWindow="15480" yWindow="2280"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="15480" yWindow="2280" windowWidth="12435" windowHeight="11505" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" state="visible" r:id="rId1"/>
@@ -51,16 +51,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -367,18 +367,18 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="14.7109375"/>
-    <col customWidth="1" max="2" min="2" width="49.85546875"/>
-    <col customWidth="1" max="3" min="3" width="17"/>
+    <col width="14.7109375" customWidth="1" min="1" max="1"/>
+    <col width="49.85546875" customWidth="1" min="2" max="2"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="19.5" r="1">
+    <row r="1" ht="19.5" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
           <t>timesheet</t>
@@ -390,23 +390,23 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19.5" r="2"/>
-    <row customHeight="1" ht="19.5" r="3">
+    <row r="2" ht="19.5" customHeight="1"/>
+    <row r="3" ht="19.5" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
           <t>month</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19.5" r="4">
+    <row r="4" ht="19.5" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19.5" r="5"/>
-    <row customHeight="1" ht="19.5" r="6">
+    <row r="5" ht="19.5" customHeight="1"/>
+    <row r="6" ht="19.5" customHeight="1">
       <c r="A6" s="1" t="inlineStr">
         <is>
           <t>project</t>
@@ -423,7 +423,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19.5" r="7">
+    <row r="7" ht="19.5" customHeight="1">
       <c r="A7" t="inlineStr">
         <is>
           <t>week 1</t>
@@ -440,7 +440,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19.5" r="8">
+    <row r="8" ht="19.5" customHeight="1">
       <c r="A8" t="inlineStr">
         <is>
           <t>week 2</t>
@@ -457,7 +457,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19.5" r="9">
+    <row r="9" ht="19.5" customHeight="1">
       <c r="A9" t="inlineStr">
         <is>
           <t>week 3</t>
@@ -474,7 +474,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19.5" r="10">
+    <row r="10" ht="19.5" customHeight="1">
       <c r="A10" t="inlineStr">
         <is>
           <t>week 4</t>
@@ -491,45 +491,45 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19.5" r="11"/>
-    <row customHeight="1" ht="19.5" r="12"/>
-    <row customHeight="1" ht="19.5" r="13"/>
-    <row customHeight="1" ht="19.5" r="14"/>
-    <row customHeight="1" ht="19.5" r="15"/>
-    <row customHeight="1" ht="19.5" r="16"/>
-    <row customHeight="1" ht="19.5" r="17"/>
-    <row customHeight="1" ht="19.5" r="18"/>
-    <row customHeight="1" ht="19.5" r="19"/>
-    <row customHeight="1" ht="19.5" r="20"/>
-    <row customHeight="1" ht="19.5" r="21"/>
-    <row customHeight="1" ht="19.5" r="22"/>
-    <row customHeight="1" ht="19.5" r="23"/>
-    <row customHeight="1" ht="19.5" r="24"/>
-    <row customHeight="1" ht="19.5" r="25"/>
-    <row customHeight="1" ht="19.5" r="26"/>
-    <row customHeight="1" ht="19.5" r="27"/>
-    <row customHeight="1" ht="19.5" r="28"/>
-    <row customHeight="1" ht="19.5" r="29"/>
-    <row customHeight="1" ht="19.5" r="30"/>
-    <row customHeight="1" ht="19.5" r="31"/>
-    <row customHeight="1" ht="19.5" r="32"/>
-    <row customHeight="1" ht="19.5" r="33"/>
-    <row customHeight="1" ht="19.5" r="34"/>
-    <row customHeight="1" ht="19.5" r="35"/>
-    <row customHeight="1" ht="19.5" r="36"/>
-    <row customHeight="1" ht="19.5" r="37"/>
-    <row customHeight="1" ht="19.5" r="38"/>
-    <row customHeight="1" ht="19.5" r="39"/>
-    <row customHeight="1" ht="19.5" r="40"/>
-    <row customHeight="1" ht="19.5" r="41"/>
-    <row customHeight="1" ht="19.5" r="42"/>
-    <row customHeight="1" ht="19.5" r="43"/>
-    <row customHeight="1" ht="19.5" r="44"/>
-    <row customHeight="1" ht="19.5" r="45"/>
-    <row customHeight="1" ht="19.5" r="46"/>
-    <row customHeight="1" ht="19.5" r="47"/>
+    <row r="11" ht="19.5" customHeight="1"/>
+    <row r="12" ht="19.5" customHeight="1"/>
+    <row r="13" ht="19.5" customHeight="1"/>
+    <row r="14" ht="19.5" customHeight="1"/>
+    <row r="15" ht="19.5" customHeight="1"/>
+    <row r="16" ht="19.5" customHeight="1"/>
+    <row r="17" ht="19.5" customHeight="1"/>
+    <row r="18" ht="19.5" customHeight="1"/>
+    <row r="19" ht="19.5" customHeight="1"/>
+    <row r="20" ht="19.5" customHeight="1"/>
+    <row r="21" ht="19.5" customHeight="1"/>
+    <row r="22" ht="19.5" customHeight="1"/>
+    <row r="23" ht="19.5" customHeight="1"/>
+    <row r="24" ht="19.5" customHeight="1"/>
+    <row r="25" ht="19.5" customHeight="1"/>
+    <row r="26" ht="19.5" customHeight="1"/>
+    <row r="27" ht="19.5" customHeight="1"/>
+    <row r="28" ht="19.5" customHeight="1"/>
+    <row r="29" ht="19.5" customHeight="1"/>
+    <row r="30" ht="19.5" customHeight="1"/>
+    <row r="31" ht="19.5" customHeight="1"/>
+    <row r="32" ht="19.5" customHeight="1"/>
+    <row r="33" ht="19.5" customHeight="1"/>
+    <row r="34" ht="19.5" customHeight="1"/>
+    <row r="35" ht="19.5" customHeight="1"/>
+    <row r="36" ht="19.5" customHeight="1"/>
+    <row r="37" ht="19.5" customHeight="1"/>
+    <row r="38" ht="19.5" customHeight="1"/>
+    <row r="39" ht="19.5" customHeight="1"/>
+    <row r="40" ht="19.5" customHeight="1"/>
+    <row r="41" ht="19.5" customHeight="1"/>
+    <row r="42" ht="19.5" customHeight="1"/>
+    <row r="43" ht="19.5" customHeight="1"/>
+    <row r="44" ht="19.5" customHeight="1"/>
+    <row r="45" ht="19.5" customHeight="1"/>
+    <row r="46" ht="19.5" customHeight="1"/>
+    <row r="47" ht="19.5" customHeight="1"/>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
@@ -540,10 +540,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -560,13 +560,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>It Worked!!</t>
-        </is>
-      </c>
-    </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -601,72 +594,389 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>week 1</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>d1</t>
+          <t>efwef</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>u1</t>
+          <t>*</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>week 2</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>d2</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>u2</t>
+          <t>week1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>week 3</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>d3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>u3</t>
+          <t>*</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>week 4</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>u4</t>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>week2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>week3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>week4</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>*</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Gui, ready to implement backend
</commit_message>
<xml_diff>
--- a/timesheets/2020_timeheets.xlsx
+++ b/timesheets/2020_timeheets.xlsx
@@ -548,7 +548,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -645,6 +645,23 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B9" s="8" t="inlineStr">
+        <is>
+          <t>weekend</t>
+        </is>
+      </c>
+      <c r="C9" s="8" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Gui,, struggling with backend
</commit_message>
<xml_diff>
--- a/timesheets/2020_timeheets.xlsx
+++ b/timesheets/2020_timeheets.xlsx
@@ -1,53 +1,105 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernard\PycharmProjects\auto_timesheet\timesheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887EB92B-3AE6-42F5-951B-6686ACF2EFFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="14790" yWindow="2205" windowWidth="12885" windowHeight="11505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="June" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="June" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+  <si>
+    <t>TIMESHEET</t>
+  </si>
+  <si>
+    <t>CNR</t>
+  </si>
+  <si>
+    <t>.Architects</t>
+  </si>
+  <si>
+    <t>MONTH:</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>NAME:</t>
+  </si>
+  <si>
+    <t>PROJECT</t>
+  </si>
+  <si>
+    <t>DESCRIPTION OF WORK</t>
+  </si>
+  <si>
+    <t>OFFICE USE</t>
+  </si>
+  <si>
+    <t>June 2020</t>
+  </si>
+  <si>
+    <t>Week3</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
       <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="18"/>
     </font>
     <font>
+      <b/>
+      <sz val="16"/>
       <name val="Bauhaus 93"/>
-      <b val="1"/>
-      <sz val="16"/>
     </font>
     <font>
+      <sz val="16"/>
       <name val="New Times Roman"/>
-      <sz val="16"/>
     </font>
     <font>
+      <b/>
+      <sz val="16"/>
       <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="16"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -63,31 +115,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="00000000"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="00000000"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="00000000"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="double">
-        <color rgb="00000000"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="00000000"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="00000000"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="00000000"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="00000000"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -96,28 +148,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -417,125 +478,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="10.5703125" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
-    <col width="22" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
-    <col width="14.28515625" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" customHeight="1" s="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>TIMESHEET</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>CNR</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>.Architects</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="19.5" customHeight="1" s="1"/>
-    <row r="3" ht="19.5" customHeight="1" s="1">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>MONTH:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>xxx</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="19.5" customHeight="1" s="1">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>NAME:</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>xxx</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="19.5" customHeight="1" s="1"/>
-    <row r="6" ht="19.5" customHeight="1" s="1">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>PROJECT</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>DESCRIPTION OF WORK</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>OFFICE USE</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="19.5" customHeight="1" s="1"/>
-    <row r="8" ht="19.5" customHeight="1" s="1"/>
-    <row r="9" ht="19.5" customHeight="1" s="1"/>
-    <row r="10" ht="19.5" customHeight="1" s="1"/>
-    <row r="11" ht="19.5" customHeight="1" s="1"/>
-    <row r="12" ht="19.5" customHeight="1" s="1"/>
-    <row r="13" ht="19.5" customHeight="1" s="1"/>
-    <row r="14" ht="19.5" customHeight="1" s="1"/>
-    <row r="15" ht="19.5" customHeight="1" s="1"/>
-    <row r="16" ht="19.5" customHeight="1" s="1"/>
-    <row r="17" ht="19.5" customHeight="1" s="1"/>
-    <row r="18" ht="19.5" customHeight="1" s="1"/>
-    <row r="19" ht="19.5" customHeight="1" s="1"/>
-    <row r="20" ht="19.5" customHeight="1" s="1"/>
-    <row r="21" ht="19.5" customHeight="1" s="1"/>
-    <row r="22" ht="19.5" customHeight="1" s="1"/>
-    <row r="23" ht="19.5" customHeight="1" s="1"/>
-    <row r="24" ht="19.5" customHeight="1" s="1"/>
-    <row r="25" ht="19.5" customHeight="1" s="1"/>
-    <row r="26" ht="19.5" customHeight="1" s="1"/>
-    <row r="27" ht="19.5" customHeight="1" s="1"/>
-    <row r="28" ht="19.5" customHeight="1" s="1"/>
-    <row r="29" ht="19.5" customHeight="1" s="1"/>
-    <row r="30" ht="19.5" customHeight="1" s="1"/>
-    <row r="31" ht="19.5" customHeight="1" s="1"/>
-    <row r="32" ht="19.5" customHeight="1" s="1"/>
-    <row r="33" ht="19.5" customHeight="1" s="1"/>
-    <row r="34" ht="19.5" customHeight="1" s="1"/>
-    <row r="35" ht="19.5" customHeight="1" s="1"/>
-    <row r="36" ht="19.5" customHeight="1" s="1"/>
-    <row r="37" ht="19.5" customHeight="1" s="1"/>
-    <row r="38" ht="19.5" customHeight="1" s="1"/>
-    <row r="39" ht="19.5" customHeight="1" s="1"/>
-    <row r="40" ht="19.5" customHeight="1" s="1"/>
-    <row r="41" ht="19.5" customHeight="1" s="1"/>
-    <row r="42" ht="19.5" customHeight="1" s="1"/>
-    <row r="43" ht="19.5" customHeight="1" s="1"/>
-    <row r="44" ht="19.5" customHeight="1" s="1"/>
-    <row r="45" ht="19.5" customHeight="1" s="1"/>
-    <row r="46" ht="19.5" customHeight="1" s="1"/>
-    <row r="47" ht="19.5" customHeight="1" s="1"/>
+    <row r="1" spans="1:3" ht="19.5" customHeight="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19.5" customHeight="1"/>
+    <row r="3" spans="1:3" ht="19.5" customHeight="1">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="19.5" customHeight="1">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="19.5" customHeight="1"/>
+    <row r="6" spans="1:3" ht="19.5" customHeight="1">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="19.5" customHeight="1"/>
+    <row r="8" spans="1:3" ht="19.5" customHeight="1"/>
+    <row r="9" spans="1:3" ht="19.5" customHeight="1"/>
+    <row r="10" spans="1:3" ht="19.5" customHeight="1"/>
+    <row r="11" spans="1:3" ht="19.5" customHeight="1"/>
+    <row r="12" spans="1:3" ht="19.5" customHeight="1"/>
+    <row r="13" spans="1:3" ht="19.5" customHeight="1"/>
+    <row r="14" spans="1:3" ht="19.5" customHeight="1"/>
+    <row r="15" spans="1:3" ht="19.5" customHeight="1"/>
+    <row r="16" spans="1:3" ht="19.5" customHeight="1"/>
+    <row r="17" ht="19.5" customHeight="1"/>
+    <row r="18" ht="19.5" customHeight="1"/>
+    <row r="19" ht="19.5" customHeight="1"/>
+    <row r="20" ht="19.5" customHeight="1"/>
+    <row r="21" ht="19.5" customHeight="1"/>
+    <row r="22" ht="19.5" customHeight="1"/>
+    <row r="23" ht="19.5" customHeight="1"/>
+    <row r="24" ht="19.5" customHeight="1"/>
+    <row r="25" ht="19.5" customHeight="1"/>
+    <row r="26" ht="19.5" customHeight="1"/>
+    <row r="27" ht="19.5" customHeight="1"/>
+    <row r="28" ht="19.5" customHeight="1"/>
+    <row r="29" ht="19.5" customHeight="1"/>
+    <row r="30" ht="19.5" customHeight="1"/>
+    <row r="31" ht="19.5" customHeight="1"/>
+    <row r="32" ht="19.5" customHeight="1"/>
+    <row r="33" ht="19.5" customHeight="1"/>
+    <row r="34" ht="19.5" customHeight="1"/>
+    <row r="35" ht="19.5" customHeight="1"/>
+    <row r="36" ht="19.5" customHeight="1"/>
+    <row r="37" ht="19.5" customHeight="1"/>
+    <row r="38" ht="19.5" customHeight="1"/>
+    <row r="39" ht="19.5" customHeight="1"/>
+    <row r="40" ht="19.5" customHeight="1"/>
+    <row r="41" ht="19.5" customHeight="1"/>
+    <row r="42" ht="19.5" customHeight="1"/>
+    <row r="43" ht="19.5" customHeight="1"/>
+    <row r="44" ht="19.5" customHeight="1"/>
+    <row r="45" ht="19.5" customHeight="1"/>
+    <row r="46" ht="19.5" customHeight="1"/>
+    <row r="47" ht="19.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -543,140 +580,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="17" customWidth="1" style="1" min="1" max="1"/>
-    <col width="48" customWidth="1" style="1" min="2" max="2"/>
-    <col width="17" customWidth="1" style="1" min="3" max="3"/>
+    <col min="1" max="1" width="17" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>TIMESHEET</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>CNR</t>
-        </is>
-      </c>
-      <c r="C1" s="6" t="inlineStr">
-        <is>
-          <t>.Architects</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>MONTH:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>June 2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>NAME:</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Bernard Muller</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="7" t="inlineStr">
-        <is>
-          <t>PROJECT</t>
-        </is>
-      </c>
-      <c r="B6" s="7" t="inlineStr">
-        <is>
-          <t>DESCRIPTION OF WORK</t>
-        </is>
-      </c>
-      <c r="C6" s="7" t="inlineStr">
-        <is>
-          <t>OFFICE USE</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="8" t="inlineStr">
-        <is>
-          <t>Week2</t>
-        </is>
-      </c>
-      <c r="B7" s="8" t="n"/>
-      <c r="C7" s="8" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="8" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="B8" s="8" t="inlineStr">
-        <is>
-          <t>Beach Villa</t>
-        </is>
-      </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>*</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="8" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="B9" s="8" t="inlineStr">
-        <is>
-          <t>weekend</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>*</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="8" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="B10" s="8" t="inlineStr">
-        <is>
-          <t>ewerwerwerw</t>
-        </is>
-      </c>
-      <c r="C10" s="8" t="inlineStr">
-        <is>
-          <t>*</t>
-        </is>
+    <row r="1" spans="1:3" ht="24.75">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>